<commit_message>
Updates in Agile Template
</commit_message>
<xml_diff>
--- a/Defect_Tracker Template_v0.1.xlsx
+++ b/Defect_Tracker Template_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://infosystechnologies-my.sharepoint.com/personal/kamaljeet_kaur01_ad_infosys_com1/Documents/Infosys/CC/Events/Oct 2021 - Mar 2022/CC2.0/Internship/Jan-Apr 2022/Artifacts/internship/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\anaconda3\envs\rasa_env\Chatbot_for_Personalized_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:101_{A9B59A9A-789B-4A89-A90D-BB9A1B756E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1529751A-99C4-4233-8104-CEB3E356847C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC51DC0F-3082-46DD-9C2B-7CA8AE7EE709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defects" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -196,7 +196,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{BC7A22E8-224C-413B-945A-EFA13D757B78}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -209,9 +211,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,9 +251,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,26 +286,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,26 +321,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -531,25 +499,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="21.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="17.5703125" style="4"/>
+    <col min="6" max="6" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="21.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="17.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -597,7 +565,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -610,7 +578,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -623,7 +591,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -636,7 +604,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -649,7 +617,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -662,7 +630,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -675,7 +643,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -688,7 +656,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -701,7 +669,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -714,7 +682,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -727,7 +695,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -740,7 +708,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -753,7 +721,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -766,7 +734,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -779,7 +747,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -792,7 +760,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -805,7 +773,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -818,7 +786,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -859,29 +827,29 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -893,6 +861,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F50FC49184C87E449886FB52439922C9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85b7e58c3d8889ba0673e7b34a193a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67b99c0-208c-4860-83e0-51466af787c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d43477c1ade21a66d9a75ba2d5aa042" ns2:_="">
     <xsd:import namespace="b67b99c0-208c-4860-83e0-51466af787c4"/>
@@ -1024,22 +1007,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191CB444-B9BF-4C91-94BD-600524521497}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1055,21 +1040,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>